<commit_message>
Fix map legend color of last interval
</commit_message>
<xml_diff>
--- a/regions_data/Ciepłownictwo/data.xlsx
+++ b/regions_data/Ciepłownictwo/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="277">
   <si>
     <t xml:space="preserve">Moc zainstalowana</t>
   </si>
@@ -73,6 +73,12 @@
     <t xml:space="preserve">Średnia cena zakupu ciepła</t>
   </si>
   <si>
+    <t xml:space="preserve">Długość sieci na mieszkańca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dolnośląskie</t>
+  </si>
+  <si>
     <t xml:space="preserve">3 526,9</t>
   </si>
   <si>
@@ -97,7 +103,7 @@
     <t xml:space="preserve">591,3</t>
   </si>
   <si>
-    <t xml:space="preserve">279 638,9</t>
+    <t xml:space="preserve">279,6389</t>
   </si>
   <si>
     <t xml:space="preserve">84,3</t>
@@ -118,6 +124,12 @@
     <t xml:space="preserve">0,03</t>
   </si>
   <si>
+    <t xml:space="preserve">0,59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kujawsko-pomorskie</t>
+  </si>
+  <si>
     <t xml:space="preserve">4 578,4</t>
   </si>
   <si>
@@ -145,7 +157,7 @@
     <t xml:space="preserve">1 335,0</t>
   </si>
   <si>
-    <t xml:space="preserve">719 014,8</t>
+    <t xml:space="preserve">719,0148</t>
   </si>
   <si>
     <t xml:space="preserve">90,2</t>
@@ -163,6 +175,12 @@
     <t xml:space="preserve">0,18</t>
   </si>
   <si>
+    <t xml:space="preserve">0,60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lubelskie</t>
+  </si>
+  <si>
     <t xml:space="preserve">2 703,3</t>
   </si>
   <si>
@@ -190,7 +208,7 @@
     <t xml:space="preserve">498,8</t>
   </si>
   <si>
-    <t xml:space="preserve">75 969,9</t>
+    <t xml:space="preserve">75,9699</t>
   </si>
   <si>
     <t xml:space="preserve">96,0</t>
@@ -208,6 +226,12 @@
     <t xml:space="preserve">0,15</t>
   </si>
   <si>
+    <t xml:space="preserve">0,48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lubuskie</t>
+  </si>
+  <si>
     <t xml:space="preserve">1 011,7</t>
   </si>
   <si>
@@ -235,7 +259,7 @@
     <t xml:space="preserve">214,4</t>
   </si>
   <si>
-    <t xml:space="preserve">109 866,1</t>
+    <t xml:space="preserve">109,8661</t>
   </si>
   <si>
     <t xml:space="preserve">73,8</t>
@@ -256,6 +280,12 @@
     <t xml:space="preserve">0,04</t>
   </si>
   <si>
+    <t xml:space="preserve">0,29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Łódzkie</t>
+  </si>
+  <si>
     <t xml:space="preserve">3 453,2</t>
   </si>
   <si>
@@ -283,7 +313,7 @@
     <t xml:space="preserve">566,1</t>
   </si>
   <si>
-    <t xml:space="preserve">368 536,6</t>
+    <t xml:space="preserve">368,5366</t>
   </si>
   <si>
     <t xml:space="preserve">85,6</t>
@@ -298,6 +328,12 @@
     <t xml:space="preserve">0,33</t>
   </si>
   <si>
+    <t xml:space="preserve">0,62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Małopolskie</t>
+  </si>
+  <si>
     <t xml:space="preserve">4 291,3</t>
   </si>
   <si>
@@ -325,7 +361,7 @@
     <t xml:space="preserve">740,3</t>
   </si>
   <si>
-    <t xml:space="preserve">376 436,1</t>
+    <t xml:space="preserve">376,4361</t>
   </si>
   <si>
     <t xml:space="preserve">85,4</t>
@@ -343,6 +379,9 @@
     <t xml:space="preserve">0,19</t>
   </si>
   <si>
+    <t xml:space="preserve">Mazowieckie</t>
+  </si>
+  <si>
     <t xml:space="preserve">10 054,7</t>
   </si>
   <si>
@@ -370,7 +409,7 @@
     <t xml:space="preserve">1 283,2</t>
   </si>
   <si>
-    <t xml:space="preserve">676 301,9</t>
+    <t xml:space="preserve">676,3019</t>
   </si>
   <si>
     <t xml:space="preserve">91,4</t>
@@ -388,6 +427,12 @@
     <t xml:space="preserve">0,02</t>
   </si>
   <si>
+    <t xml:space="preserve">0,56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opolskie</t>
+  </si>
+  <si>
     <t xml:space="preserve">1 576,0</t>
   </si>
   <si>
@@ -415,7 +460,7 @@
     <t xml:space="preserve">368,6</t>
   </si>
   <si>
-    <t xml:space="preserve">161 789,1</t>
+    <t xml:space="preserve">161,7891</t>
   </si>
   <si>
     <t xml:space="preserve">88,1</t>
@@ -430,6 +475,12 @@
     <t xml:space="preserve">0,36</t>
   </si>
   <si>
+    <t xml:space="preserve">0,61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Podkarpackie</t>
+  </si>
+  <si>
     <t xml:space="preserve">1 605,7</t>
   </si>
   <si>
@@ -457,7 +508,7 @@
     <t xml:space="preserve">308,5</t>
   </si>
   <si>
-    <t xml:space="preserve">60 054,4</t>
+    <t xml:space="preserve">60,0544</t>
   </si>
   <si>
     <t xml:space="preserve">95,0</t>
@@ -478,6 +529,12 @@
     <t xml:space="preserve">0,05</t>
   </si>
   <si>
+    <t xml:space="preserve">0,35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Podlaskie</t>
+  </si>
+  <si>
     <t xml:space="preserve">723,8</t>
   </si>
   <si>
@@ -505,7 +562,7 @@
     <t xml:space="preserve">245,3</t>
   </si>
   <si>
-    <t xml:space="preserve">57 662,7</t>
+    <t xml:space="preserve">57,6627</t>
   </si>
   <si>
     <t xml:space="preserve">83,9</t>
@@ -523,6 +580,12 @@
     <t xml:space="preserve">0,16</t>
   </si>
   <si>
+    <t xml:space="preserve">0,53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pomorskie</t>
+  </si>
+  <si>
     <t xml:space="preserve">3 734,4</t>
   </si>
   <si>
@@ -550,7 +613,7 @@
     <t xml:space="preserve">1 055,7</t>
   </si>
   <si>
-    <t xml:space="preserve">302 051,6</t>
+    <t xml:space="preserve">302,0516</t>
   </si>
   <si>
     <t xml:space="preserve">104,3</t>
@@ -559,6 +622,12 @@
     <t xml:space="preserve">0,22</t>
   </si>
   <si>
+    <t xml:space="preserve">0,69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Śląskie</t>
+  </si>
+  <si>
     <t xml:space="preserve">10 505,8</t>
   </si>
   <si>
@@ -586,7 +655,7 @@
     <t xml:space="preserve">1 992,6</t>
   </si>
   <si>
-    <t xml:space="preserve">881 454,7</t>
+    <t xml:space="preserve">881,4547</t>
   </si>
   <si>
     <t xml:space="preserve">82,2</t>
@@ -598,12 +667,15 @@
     <t xml:space="preserve">90,3</t>
   </si>
   <si>
-    <t xml:space="preserve">0,29</t>
-  </si>
-  <si>
     <t xml:space="preserve">0,13</t>
   </si>
   <si>
+    <t xml:space="preserve">0,68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Świętokrzyskie</t>
+  </si>
+  <si>
     <t xml:space="preserve">1 237,5</t>
   </si>
   <si>
@@ -631,7 +703,7 @@
     <t xml:space="preserve">418,0</t>
   </si>
   <si>
-    <t xml:space="preserve">19 355,0</t>
+    <t xml:space="preserve">19,355</t>
   </si>
   <si>
     <t xml:space="preserve">77,4</t>
@@ -649,6 +721,12 @@
     <t xml:space="preserve">0,06</t>
   </si>
   <si>
+    <t xml:space="preserve">0,37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warmińsko-mazurskie</t>
+  </si>
+  <si>
     <t xml:space="preserve">1 461,7</t>
   </si>
   <si>
@@ -676,7 +754,7 @@
     <t xml:space="preserve">514,6</t>
   </si>
   <si>
-    <t xml:space="preserve">80 012,8</t>
+    <t xml:space="preserve">80,0128</t>
   </si>
   <si>
     <t xml:space="preserve">73,2</t>
@@ -685,7 +763,10 @@
     <t xml:space="preserve">110,5</t>
   </si>
   <si>
-    <t xml:space="preserve">0,37</t>
+    <t xml:space="preserve">0,46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wielkopolskie</t>
   </si>
   <si>
     <t xml:space="preserve">3 372,1</t>
@@ -715,7 +796,7 @@
     <t xml:space="preserve">1 224,3</t>
   </si>
   <si>
-    <t xml:space="preserve">170 765,2</t>
+    <t xml:space="preserve">170,7652</t>
   </si>
   <si>
     <t xml:space="preserve">84,6</t>
@@ -727,6 +808,9 @@
     <t xml:space="preserve">107,1</t>
   </si>
   <si>
+    <t xml:space="preserve">Zachodniopomorskie</t>
+  </si>
+  <si>
     <t xml:space="preserve">2 212,2</t>
   </si>
   <si>
@@ -754,7 +838,7 @@
     <t xml:space="preserve">606,0</t>
   </si>
   <si>
-    <t xml:space="preserve">133 115,6</t>
+    <t xml:space="preserve">133,1156</t>
   </si>
   <si>
     <t xml:space="preserve">87,9</t>
@@ -764,18 +848,24 @@
   </si>
   <si>
     <t xml:space="preserve">124,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,51</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="#,##0"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
+    <numFmt numFmtId="169" formatCode="0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -807,6 +897,13 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -822,7 +919,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -835,6 +932,13 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -863,7 +967,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -892,6 +996,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -909,929 +1029,1077 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q22" activeCellId="0" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.25"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.7040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="6" style="0" width="8.75"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.4948979591837"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.4897959183673"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.5714285714286"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.8163265306122"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.4336734693878"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="26.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="23.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>16</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="6" t="n">
         <v>22666</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="J2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="L2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="M2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="N2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="O2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="P2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="8" t="n">
         <v>61</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" s="10" t="n">
+        <v>2908457</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="0" t="n">
+      <c r="R3" s="8" t="n">
         <v>59.69</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="T3" s="10" t="n">
+        <v>2089992</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>48</v>
+      <c r="A4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="J4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4" s="0" t="n">
+      <c r="K4" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="8" t="n">
         <v>52.4</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="T4" s="10" t="n">
+        <v>2147746</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>63</v>
+      <c r="A5" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>67</v>
+        <v>72</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="P5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Q5" s="0" t="n">
+      <c r="J5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="R5" s="8" t="n">
         <v>61.43</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="T5" s="10" t="n">
+        <v>1020307</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>79</v>
+      <c r="A6" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>83</v>
+        <v>90</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" s="8" t="n">
         <v>53.96</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="T6" s="10" t="n">
+        <v>2504136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>93</v>
+      <c r="A7" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>97</v>
+        <v>106</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q7" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R7" s="8" t="n">
         <v>56.7</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="T7" s="10" t="n">
+        <v>3368336</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>108</v>
+      <c r="A8" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>112</v>
+        <v>122</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="K8" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="P8" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q8" s="0" t="n">
+      <c r="Q8" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="R8" s="8" t="n">
         <v>50.85</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="T8" s="10" t="n">
+        <v>5334511</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>123</v>
+      <c r="A9" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>127</v>
+        <v>139</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q9" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="R9" s="8" t="n">
         <v>63.06</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="T9" s="10" t="n">
+        <v>1000858</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>137</v>
+      <c r="A10" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>153</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>141</v>
+        <v>155</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q10" s="0" t="n">
+        <v>160</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="R10" s="8" t="n">
         <v>58.35</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="T10" s="10" t="n">
+        <v>2129187</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>153</v>
+      <c r="A11" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>157</v>
+        <v>173</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>175</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q11" s="0" t="n">
+        <v>178</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="R11" s="8" t="n">
         <v>57.44</v>
+      </c>
+      <c r="S11" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="T11" s="10" t="n">
+        <v>1191918</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>168</v>
+      <c r="A12" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>188</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>172</v>
+        <v>190</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>192</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q12" s="0" t="n">
+        <v>195</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="R12" s="8" t="n">
         <v>58.92</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="T12" s="10" t="n">
+        <v>2302077</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>180</v>
+      <c r="A13" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>202</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>184</v>
+        <v>204</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>206</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>186</v>
+        <v>208</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q13" s="0" t="n">
+        <v>209</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="R13" s="8" t="n">
         <v>57.78</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="T13" s="10" t="n">
+        <v>4585924</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>195</v>
+      <c r="A14" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>218</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>199</v>
+        <v>220</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>222</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q14" s="0" t="n">
+        <v>225</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="R14" s="8" t="n">
         <v>56.36</v>
+      </c>
+      <c r="S14" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="T14" s="10" t="n">
+        <v>1263176</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>210</v>
+      <c r="A15" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>214</v>
+        <v>237</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q15" s="0" t="n">
+        <v>242</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="R15" s="8" t="n">
         <v>57.42</v>
+      </c>
+      <c r="S15" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="T15" s="10" t="n">
+        <v>1443967</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>223</v>
+      <c r="A16" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>249</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>224</v>
+        <v>250</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>227</v>
+        <v>251</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>253</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>229</v>
+        <v>255</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="K16" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q16" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="L16" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q16" s="0" t="n">
+      <c r="R16" s="8" t="n">
         <v>60.9</v>
+      </c>
+      <c r="S16" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="T16" s="10" t="n">
+        <v>3472579</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>236</v>
+      <c r="A17" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>263</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>237</v>
+        <v>264</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>240</v>
+        <v>265</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>267</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>242</v>
+        <v>269</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q17" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="R17" s="8" t="n">
         <v>61.31</v>
+      </c>
+      <c r="S17" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="T17" s="10" t="n">
+        <v>1715431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>